<commit_message>
Affichage des informations des universités
</commit_message>
<xml_diff>
--- a/Data/data_entreprises.xlsx
+++ b/Data/data_entreprises.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axell\Documents\Docs\Polytech\FI4\DATA732 - Analyse et Visualisation\DATA732_Projet-UNITA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B88F1D-66EA-472E-914A-2BB64C16B8AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759D0B93-1107-4B95-9FF1-C6AFA831873A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5130" yWindow="-16320" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RIS" sheetId="1" r:id="rId1"/>
@@ -11922,7 +11922,7 @@
   <dimension ref="A2:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
@@ -13583,7 +13583,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="319" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -13760,7 +13760,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="406" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
@@ -18169,7 +18169,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="225" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="225" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="A21" s="125" t="s">
         <v>20</v>
       </c>
@@ -18199,7 +18199,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="231" customFormat="1" ht="188.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="231" customFormat="1" ht="203" x14ac:dyDescent="0.25">
       <c r="A22" s="125" t="s">
         <v>20</v>
       </c>
@@ -18237,7 +18237,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="231" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="231" customFormat="1" ht="145" x14ac:dyDescent="0.25">
       <c r="A23" s="125" t="s">
         <v>20</v>
       </c>
@@ -23589,7 +23589,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A15" s="73" t="s">
         <v>20</v>
       </c>
@@ -23701,7 +23701,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="116" x14ac:dyDescent="0.25">
       <c r="A19" s="73" t="s">
         <v>20</v>
       </c>
@@ -23925,7 +23925,7 @@
         <v>1938</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="130.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="145" x14ac:dyDescent="0.25">
       <c r="A27" s="73" t="s">
         <v>20</v>
       </c>
@@ -24120,7 +24120,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="72.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="87" x14ac:dyDescent="0.25">
       <c r="A34" s="73" t="s">
         <v>20</v>
       </c>

</xml_diff>